<commit_message>
modules require file adde
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding-folder\python\birthdaywisher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding-folder\python\Projects\Birthday-wisher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F79B4D-2078-496C-AB05-FE8C96A571B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4318ADC-D5ED-454B-9B85-255D3A9CFA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -37,25 +37,28 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Himanshu Bedi</t>
+  </si>
+  <si>
+    <t>Happy Birthday</t>
+  </si>
+  <si>
+    <t>2020,2022</t>
+  </si>
+  <si>
     <t>Ankit</t>
   </si>
   <si>
-    <t>Happy Birthday</t>
-  </si>
-  <si>
     <t>ankitj.cs.20@nitj.ac.in</t>
   </si>
   <si>
-    <t>Himanshu Bedi</t>
-  </si>
-  <si>
-    <t>himanshub.cs.20@nitj.in</t>
-  </si>
-  <si>
     <t>Harsh Dhiman</t>
   </si>
   <si>
     <t>harshd.cs.20@nitj.ac.in</t>
+  </si>
+  <si>
+    <t>himanshub.cs.20@nitj.ac.in</t>
   </si>
 </sst>
 </file>
@@ -63,9 +66,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +80,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,17 +122,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,13 +439,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -453,7 +470,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>44926</v>
@@ -461,16 +478,16 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>2020</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>44562</v>
@@ -481,8 +498,8 @@
       <c r="D3">
         <v>2020</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -498,11 +515,16 @@
       <c r="D4">
         <v>2020</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8F1F521A-0F12-4923-A1C5-41F839923D9D}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{54AF639D-542A-41E9-B87E-BFF41811DD7A}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{44CCC34F-AC8D-4442-A960-0B72AC43E83A}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>